<commit_message>
primul commit on git cmd 15.32
</commit_message>
<xml_diff>
--- a/Parameters--do not translate list--2023_ambiguous .xlsx
+++ b/Parameters--do not translate list--2023_ambiguous .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mboros\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D24B791-C8A9-4524-A444-7F8F4E9C56D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9AC346-6EAE-4FC4-9D32-06DD6EC64DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34830" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{D5A22007-63F0-4073-B14E-DAC0B9B386F1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3071" uniqueCount="2872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="2873">
   <si>
     <t xml:space="preserve">A </t>
   </si>
@@ -26830,6 +26830,9 @@
   </si>
   <si>
     <t>comentariu local _27.10</t>
+  </si>
+  <si>
+    <t>alt comentariu 27.10 ora 15.31</t>
   </si>
 </sst>
 </file>
@@ -27299,7 +27302,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27376,6 +27379,9 @@
       <c r="E4" t="s">
         <v>2850</v>
       </c>
+      <c r="F4" t="s">
+        <v>2872</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">

</xml_diff>